<commit_message>
security Test configuration modified
</commit_message>
<xml_diff>
--- a/Input/Automation_input.xlsx
+++ b/Input/Automation_input.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CMMP_Automation\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\zapkra\Nallas_demoproject\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347E729B-9CD7-4F91-A200-0CE2580BB4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9904F3E3-BA0A-42C4-82BF-BBA96479E551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{9B9FB4DD-39F9-4DD6-9D49-788E00E4870F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9B9FB4DD-39F9-4DD6-9D49-788E00E4870F}"/>
   </bookViews>
   <sheets>
     <sheet name="Execution" sheetId="1" r:id="rId1"/>
-    <sheet name="input action" sheetId="4" r:id="rId2"/>
-    <sheet name="TC_100" sheetId="2" r:id="rId3"/>
-    <sheet name="TC_101" sheetId="3" r:id="rId4"/>
+    <sheet name="Configuration" sheetId="5" r:id="rId2"/>
+    <sheet name="input action" sheetId="4" r:id="rId3"/>
+    <sheet name="TC_100" sheetId="2" r:id="rId4"/>
+    <sheet name="TC_101" sheetId="3" r:id="rId5"/>
+    <sheet name="TC_102" sheetId="6" r:id="rId6"/>
+    <sheet name="TC_103" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="93">
   <si>
     <t>TestcaseId</t>
   </si>
@@ -66,42 +69,6 @@
     <t>Xpath</t>
   </si>
   <si>
-    <t>Http://www.amazon.in</t>
-  </si>
-  <si>
-    <t>//a[@data-csa-c-content-id='nav_cs_mobiles'][contains(text(),'Mobiles')]</t>
-  </si>
-  <si>
-    <t>//a[contains(text(),'Accessories')][@role='tab']</t>
-  </si>
-  <si>
-    <t>click mobile category</t>
-  </si>
-  <si>
-    <t>click Accessories tab</t>
-  </si>
-  <si>
-    <t>open accessories which is lesser than 500.</t>
-  </si>
-  <si>
-    <t>//span[@class='a-price-whole']</t>
-  </si>
-  <si>
-    <t>Move control to new tab</t>
-  </si>
-  <si>
-    <t>Add product to cart</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'Add to Cart')][@id='submit.add-to-cart-announce']</t>
-  </si>
-  <si>
-    <t>Verify cart count</t>
-  </si>
-  <si>
-    <t>//div[@id='nav-cart-count-container']/span[@id='nav-cart-count']</t>
-  </si>
-  <si>
     <t>To add mobile Access</t>
   </si>
   <si>
@@ -109,12 +76,6 @@
   </si>
   <si>
     <t>Browser</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Firefox</t>
   </si>
   <si>
     <t>LaunchWebsite</t>
@@ -294,6 +255,75 @@
   <si>
     <t>used to verify text was not contains
 Input_Data: Enter input data</t>
+  </si>
+  <si>
+    <t>APIKEY</t>
+  </si>
+  <si>
+    <t>1gtc2jti2if23npr7uk82g64dm</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>ZAPTOOL_Location</t>
+  </si>
+  <si>
+    <t>C:\Program Files\ZAP\Zed Attack Proxy\zap.bat</t>
+  </si>
+  <si>
+    <t>https://nallas.com/</t>
+  </si>
+  <si>
+    <t>//li/a[contains(text(),'Services')]</t>
+  </si>
+  <si>
+    <t>//li/a[contains(text(),'Data Engineering')]</t>
+  </si>
+  <si>
+    <t>//li/a[contains(text(),'Contact Us')][@class='hfe-menu-item']</t>
+  </si>
+  <si>
+    <t>click service menu</t>
+  </si>
+  <si>
+    <t>click data engineering menu</t>
+  </si>
+  <si>
+    <t>click contact us menu</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'Submit Inquiry')]</t>
+  </si>
+  <si>
+    <t>//input[@id='wpforms-3789-field_2']</t>
+  </si>
+  <si>
+    <t>Enter value in first name</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>//input[@id='wpforms-3789-field_4']</t>
+  </si>
+  <si>
+    <t>Enter value in last name</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>Security_scan</t>
   </si>
 </sst>
 </file>
@@ -681,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D15300-7BA8-4C13-A480-70ED76A1B05C}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,6 +723,7 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="17.1796875" customWidth="1"/>
     <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -706,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,27 +745,55 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -743,11 +802,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D9E7CD-4706-49C1-8946-D8EA158549E7}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D0E214-C12E-4B6C-83F6-39FC3A8DF824}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,7 +858,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -766,242 +866,242 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1010,12 +1110,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C02876-3B64-409D-A3D2-DF78F2C91C55}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,28 +1157,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -1089,34 +1189,32 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2000</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D5" s="3"/>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -1127,49 +1225,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1185,7 +1249,7 @@
           <x14:formula1>
             <xm:f>'input action'!$A$3:$A$32</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C9</xm:sqref>
+          <xm:sqref>C2:C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1193,12 +1257,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94E46F7-DD03-4D45-B04A-1BB850E3B038}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1207,7 +1271,7 @@
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="32.6328125" customWidth="1"/>
     <col min="4" max="4" width="28.26953125" customWidth="1"/>
-    <col min="5" max="5" width="25.90625" customWidth="1"/>
+    <col min="5" max="5" width="43.90625" customWidth="1"/>
     <col min="6" max="6" width="24.1796875" customWidth="1"/>
     <col min="7" max="7" width="23.26953125" customWidth="1"/>
   </cols>
@@ -1240,28 +1304,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -1272,34 +1336,32 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2000</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D5" s="3"/>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -1309,48 +1371,48 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
+      <c r="B6" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
@@ -1358,7 +1420,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{C6146C7A-2575-47AA-9746-09874F0A6F53}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6375B1FD-98A5-49CB-B2DF-07B925F9A1B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1374,4 +1436,366 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CD24B9-6A35-4F51-92DE-AB71D93EE7B6}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="32.6328125" customWidth="1"/>
+    <col min="4" max="4" width="28.26953125" customWidth="1"/>
+    <col min="5" max="5" width="43.90625" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0C9BFD9C-C867-4E89-8F70-53F24A21A86F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5D83F52-08C9-4BB5-9973-57F5D9FFEB9B}">
+          <x14:formula1>
+            <xm:f>'input action'!$A$3:$A$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D3AB5A-1CB6-44F4-9DE9-4B465F268EB0}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="32.6328125" customWidth="1"/>
+    <col min="4" max="4" width="28.26953125" customWidth="1"/>
+    <col min="5" max="5" width="43.90625" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{AE03CD1A-972B-4E62-9AD4-C7112BF37538}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83946C29-B3F6-4D2E-97C6-FEFCD0E007D1}">
+          <x14:formula1>
+            <xm:f>'input action'!$A$3:$A$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>